<commit_message>
Add code to generate figures with upper and lower confidence intervals, plus removed old code that I am no longer using.
</commit_message>
<xml_diff>
--- a/R/Output/Summary_table.xlsx
+++ b/R/Output/Summary_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kc1-my.sharepoint.com/personal/adavid_kingcounty_gov/Documents/Desktop/Projects/Green River PIT tag study/GreenRiverPIT/R/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{00374869-D6A5-40C5-B914-8D1028BEEB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FF86DA8-981E-4ECB-9620-E88AC3F09134}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{00374869-D6A5-40C5-B914-8D1028BEEB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F52803C1-0D7D-4DCD-A855-90B5CF3B845E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CD984D28-82D8-4117-A6FB-B5EC6BA97157}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CD984D28-82D8-4117-A6FB-B5EC6BA97157}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_table" sheetId="1" r:id="rId1"/>
@@ -943,9 +943,9 @@
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>